<commit_message>
Add praesi for milestone 3
</commit_message>
<xml_diff>
--- a/Projektplanung/Gantt-DiagrammMilestone2.xlsx
+++ b/Projektplanung/Gantt-DiagrammMilestone2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7631E880-3B02-4F30-B366-A6B5758A8556}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFE65B9-B165-4630-B9B4-962D2DAF399D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagrammdaten" sheetId="1" r:id="rId1"/>
@@ -337,9 +337,6 @@
     <t>Silvester/Neujahr</t>
   </si>
   <si>
-    <t>Interaktionskomponenten (Checkboxen)</t>
-  </si>
-  <si>
     <t>Logik für Interaktionskomponenten</t>
   </si>
   <si>
@@ -362,6 +359,9 @@
   </si>
   <si>
     <t>Präsentation erstellen</t>
+  </si>
+  <si>
+    <t>Interaktionskomponenten erweitern</t>
   </si>
 </sst>
 </file>
@@ -967,13 +967,6 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
@@ -1027,6 +1020,13 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1227,7 +1227,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5865397-A356-4CEA-A367-389B5D0BA0AA}" type="CELLRANGE">
+                    <a:fld id="{5A7B60DF-8558-44A9-AAB3-F88A5AA4B9AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1260,7 +1260,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5CFC277-3E10-4168-9DA1-456CB2C4FCC1}" type="CELLRANGE">
+                    <a:fld id="{61A1578D-817E-4405-902E-DAB666FA33E0}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1294,7 +1294,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A36DA42E-77A5-4D9F-B6C6-C6473BFBFC28}" type="CELLRANGE">
+                    <a:fld id="{88FFD4E1-731E-44D3-AB06-FD844736957B}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1328,7 +1328,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32F327B8-DA23-4E6D-98E7-C1D415570327}" type="CELLRANGE">
+                    <a:fld id="{B58D28A9-A002-464F-83A9-DD61D80A36D8}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1362,7 +1362,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{937272DF-2036-45BC-8EA5-ACF5E3BDA43F}" type="CELLRANGE">
+                    <a:fld id="{46E3B7D7-6628-4876-8667-8BB523CF089C}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1396,7 +1396,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5FD853D-36E4-4EA8-935A-11FB92540ED8}" type="CELLRANGE">
+                    <a:fld id="{CCEE4A0E-435B-4D37-AC56-073C3BC1F6D7}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1430,7 +1430,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8C9D870-1682-41E2-A8CC-51CC5A39E4C3}" type="CELLRANGE">
+                    <a:fld id="{BEE2C36E-6244-46E2-B1E1-783034C83FF4}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1695,7 +1695,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8766CF12-3059-43E8-A551-79B43DE1FC42}" type="CELLRANGE">
+                    <a:fld id="{F34D96BE-2400-4B54-959F-EC8F4607F3C1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1818,10 +1818,10 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>44178</c:v>
+                  <c:v>44179</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44178</c:v>
+                  <c:v>44179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1892,7 +1892,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4EF67EEC-3742-4221-9E33-A9DDE01E62A0}" type="CELLRANGE">
+                    <a:fld id="{0AB07EE6-7887-4850-8F4B-7E872B463400}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1925,7 +1925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B54FF8E6-DC92-4BF2-B42E-E315D814F50D}" type="CELLRANGE">
+                    <a:fld id="{84E1B2D6-1331-4A9A-8664-BE60CEE8F41B}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1959,7 +1959,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EACAF758-D387-4759-B8BB-58E587202ADC}" type="CELLRANGE">
+                    <a:fld id="{E1265B92-B07C-469D-A5C7-6E867E94FE99}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1993,7 +1993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B633CB72-33A2-403C-94AC-916954932F9F}" type="CELLRANGE">
+                    <a:fld id="{3E61EEC3-0A33-48C4-9F57-628BA5F38806}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2027,7 +2027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB180FD7-4EE8-4383-A80B-046EB87ABE4D}" type="CELLRANGE">
+                    <a:fld id="{E0244D05-E1E9-4C21-A8BE-D65A5489D80E}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2061,7 +2061,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4E5C1D5-6E83-402A-BAD6-23F3DFC4B8D0}" type="CELLRANGE">
+                    <a:fld id="{362AD641-34EE-4187-8481-791318FCD9A8}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2095,7 +2095,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B364A0CB-7726-4EE6-98A7-F6116D62C5FB}" type="CELLRANGE">
+                    <a:fld id="{A57AC99F-B660-4975-BE00-4B6DC7E4A4FB}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2129,7 +2129,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70705302-4478-4B04-996D-F4E456C913DD}" type="CELLRANGE">
+                    <a:fld id="{190B5664-1308-4617-BCD1-B475AB5EAD34}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2163,7 +2163,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0645D3D3-A17F-429F-BA10-9579F2DE0C80}" type="CELLRANGE">
+                    <a:fld id="{AB7843B7-067E-4678-928B-94BCD9DC5BD7}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2197,7 +2197,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A146C185-9D34-4EA0-B089-48189317B3B3}" type="CELLRANGE">
+                    <a:fld id="{6D195DD8-79EE-495A-9977-897116F46417}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2231,7 +2231,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{711D540C-18FE-41D8-AA68-27118C82D612}" type="CELLRANGE">
+                    <a:fld id="{807C3471-5DC9-449D-A251-FD8D914A754E}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2265,7 +2265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27B10FE8-9C86-45BC-9553-1E8639AA2B0B}" type="CELLRANGE">
+                    <a:fld id="{A1FAF0AF-9FC9-449E-A0FF-98066DEA8231}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2299,7 +2299,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECED52FF-0A47-4F0C-99E8-3902B8761E00}" type="CELLRANGE">
+                    <a:fld id="{21D79DA9-1BD8-4F1C-AB34-59049883D7C0}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2333,7 +2333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B162BF3-0526-41DF-9D5B-B1DC0A139EF2}" type="CELLRANGE">
+                    <a:fld id="{BC584875-4625-43BC-A01D-BBB9D0C40298}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2367,7 +2367,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18867DA4-A24B-403F-A22F-BCB9085A19FD}" type="CELLRANGE">
+                    <a:fld id="{E21681EB-99A2-4340-BEC4-4FFE30A20354}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -3355,13 +3355,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>8844</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>291466</xdr:rowOff>
+      <xdr:rowOff>291467</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>2019300</xdr:rowOff>
+      <xdr:rowOff>1924050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3495,16 +3495,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Vorgänge" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Vorgänge" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET(Diagrammdaten!$H6,ScrollSchrittweite[Scrollschrittweite],0,1,1))=0,"",IF(OR(OFFSET(Diagrammdaten!$I6,ScrollSchrittweite[Scrollschrittweite],0,1,1)&lt;=$B$12,OFFSET(Diagrammdaten!$H6,ScrollSchrittweite[Scrollschrittweite],0,1,1)&gt;=($B$11-$D$11)),INDEX(Aufgaben[],OFFSET(Diagrammdaten!$G6,ScrollSchrittweite[Scrollschrittweite],0,1,1),4),"")),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Anfangsdatum" dataCellStyle="Datum">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamischeAufgabenDaten[[#This Row],[Vorgänge]])=0,$B$11,INDEX(Aufgaben[],OFFSET(Diagrammdaten!$G6,ScrollSchrittweite[Scrollschrittweite],0,1,1),2)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Vorgangsdauer in Tagen" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Vorgangsdauer in Tagen" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamischeAufgabenDaten[[#This Row],[Vorgänge]])=0,0,IF(AND(Diagrammdaten!$H6&lt;=$B$12,Diagrammdaten!$I6&gt;=$B$12),ABS(OFFSET(Diagrammdaten!$H6,ScrollSchrittweite[Scrollschrittweite],0,1,1)-$B$12)+1,OFFSET(Diagrammdaten!$K6,ScrollSchrittweite[Scrollschrittweite],0,1,1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Position" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Position" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamischeAufgabenDaten[[#This Row],[Vorgänge]])=0,"",ROW($A1)),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3521,10 +3521,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="HeuteHervorhebung" displayName="HeuteHervorhebung" ref="B3:C5" totalsRowShown="0">
   <autoFilter ref="B3:C5" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Heute-Hervorhebung X-Koordinate" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Heute-Hervorhebung X-Koordinate" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(IF(TODAY()&lt;MIN(DynamischeAufgabenDaten[Anfangsdatum]),MIN($B$11,MIN(DynamischeAufgabenDaten[Anfangsdatum])),TODAY()),TODAY())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Y-Koordinate" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Y-Koordinate" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(IF(Nachverfolgen_Heute="Ja",IF(TODAY()&lt;MIN(DynamischeAufgabenDaten[Anfangsdatum]),0,9),0),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3545,13 +3545,13 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Meilensteine" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Meilensteine" dataDxfId="6">
       <calculatedColumnFormula>IFERROR(IF(LEN(Diagrammdaten!D6)=0,"",IF(AND(Diagrammdaten!D6&lt;=$B$12,Diagrammdaten!D6&gt;=$B$11-$D$11),Diagrammdaten!E6,"")),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Datum" dataDxfId="6" dataCellStyle="Datum">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Datum" dataDxfId="5" dataCellStyle="Datum">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamischeMeilensteinDaten[[#This Row],[Meilensteine]])=0,$B$12,Diagrammdaten!$D6),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Basisplan" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Basisplan" dataDxfId="4">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamischeMeilensteinDaten[[#This Row],[Meilensteine]])=0,"",Diagrammdaten!$C6),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3560,12 +3560,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="ScrollSchrittweite" displayName="ScrollSchrittweite" ref="B7:B8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="ScrollSchrittweite" displayName="ScrollSchrittweite" ref="B7:B8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="B7:B8" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Scrollschrittweite" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Scrollschrittweite" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Date Tracking Gantt Chart" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3580,7 +3580,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="DiagrammBereich" displayName="DiagrammBereich" ref="B10:B12" totalsRowShown="0">
   <autoFilter ref="B10:B12" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Diagrammbereich" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Diagrammbereich" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(IF(LEN(#REF!)=0,End_Date+15,MIN(#REF!)+15),TODAY())</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3900,8 +3900,8 @@
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4177,7 +4177,7 @@
         <v>44229</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11" s="11">
         <v>6</v>
@@ -4234,7 +4234,7 @@
         <v>44177</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K13" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4256,7 +4256,7 @@
         <v>44178</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K14" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4278,7 +4278,7 @@
         <v>44181</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4300,7 +4300,7 @@
         <v>44181</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K16" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4433,7 +4433,7 @@
         <v>44203</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="K22" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4451,7 +4451,7 @@
         <v>44209</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K23" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4469,7 +4469,7 @@
         <v>44214</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K24" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4487,7 +4487,7 @@
         <v>44223</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K25" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4508,7 +4508,7 @@
         <v>44229</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K26" s="25">
         <f>IFERROR(IF(LEN(Aufgaben[[#This Row],[Anfangsdatum]])=0,"",(INT(Aufgaben[[#This Row],[Enddatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))-(INT(Aufgaben[[#This Row],[Anfangsdatum]])-INT(Aufgaben[[#This Row],[Anfangsdatum]]))+1),"")</f>
@@ -4582,7 +4582,7 @@
   </sheetPr>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
@@ -4620,7 +4620,7 @@
     <row r="3" spans="1:18" ht="162.4" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="C2:O2">
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>#REF!&lt;=TODAY()+7</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4719,7 +4719,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f ca="1">IFERROR(IF(TODAY()&lt;MIN(DynamischeAufgabenDaten[Anfangsdatum]),MIN($B$11,MIN(DynamischeAufgabenDaten[Anfangsdatum])),TODAY()),TODAY())</f>
-        <v>44178</v>
+        <v>44179</v>
       </c>
       <c r="C4" s="3">
         <f ca="1">IFERROR(IF(Nachverfolgen_Heute="Ja",IF(TODAY()&lt;MIN(DynamischeAufgabenDaten[Anfangsdatum]),0,9),0),0)</f>
@@ -4729,7 +4729,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <f ca="1">IFERROR(IF(TODAY()&lt;MIN(DynamischeAufgabenDaten[Anfangsdatum]),MIN($B$11,MIN(DynamischeAufgabenDaten[Anfangsdatum])),TODAY()),TODAY())</f>
-        <v>44178</v>
+        <v>44179</v>
       </c>
       <c r="C5" s="3">
         <f ca="1">IFERROR(IF(Nachverfolgen_Heute="Ja",IF(TODAY()&lt;MIN(DynamischeAufgabenDaten[Anfangsdatum]),0,9),0),0)</f>

</xml_diff>